<commit_message>
Kto Pchelok Uvazhaet - UPDATE +GUI
</commit_message>
<xml_diff>
--- a/ЛМЕ-УКПК-2021.xlsx
+++ b/ЛМЕ-УКПК-2021.xlsx
@@ -2361,7 +2361,11 @@
       <c r="A26" s="23" t="n">
         <v>19</v>
       </c>
-      <c r="B26" s="26" t="n"/>
+      <c r="B26" s="26" t="inlineStr">
+        <is>
+          <t>9435</t>
+        </is>
+      </c>
       <c r="C26" s="14" t="n"/>
       <c r="D26" s="15" t="n"/>
       <c r="E26" s="15" t="n"/>
@@ -2374,7 +2378,11 @@
         <v>20</v>
       </c>
       <c r="B27" s="17" t="n"/>
-      <c r="C27" s="18" t="n"/>
+      <c r="C27" s="18" t="inlineStr">
+        <is>
+          <t>73.3315</t>
+        </is>
+      </c>
       <c r="D27" s="19" t="n"/>
       <c r="E27" s="19" t="n"/>
       <c r="F27" s="17" t="n"/>

</xml_diff>